<commit_message>
Enhance user registration process by adding email, course, class name, and roll number fields; implement validation for input formats.
</commit_message>
<xml_diff>
--- a/jack-django/register.xlsx
+++ b/jack-django/register.xlsx
@@ -1,57 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Default Event"/>
+    <sheet name="Default Event" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>saad</t>
-  </si>
-  <si>
-    <t>9347151331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sahil
-</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,24 +46,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -375,42 +413,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Mobile</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>saad</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>9347151331</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sahil
+</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sahil</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1122990088</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sameer</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0000000000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>mdshaiksahil0510@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CSE IOT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CSEIOT</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>161023749019</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>masood</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7981842202</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2005syedmasood@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>BE</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>161023733094</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance chat interface by adding a scrollable table container, implementing commands for displaying and clearing messages, and adjusting message rendering for better HTML support.
</commit_message>
<xml_diff>
--- a/jack-django/register.xlsx
+++ b/jack-django/register.xlsx
@@ -1,33 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Default Event" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Test"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mobile no.</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Roll no.</t>
+  </si>
+  <si>
+    <t>SAHIL</t>
+  </si>
+  <si>
+    <t>9347151331</t>
+  </si>
+  <si>
+    <t>mdshaiksahil0510@gmail.com</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>CSE IOT</t>
+  </si>
+  <si>
+    <t>161023749019</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,86 +87,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,134 +392,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Mobile</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>saad</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>9347151331</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sahil
-</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sahil</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1122990088</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sameer</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0000000000</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>mdshaiksahil0510@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CSE IOT</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CSEIOT</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>161023749019</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>masood</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7981842202</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2005syedmasood@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>BE</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>161023733094</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance registration process by updating bot responses, adding input validation, and improving message prompts; include new commands for user interaction.
</commit_message>
<xml_diff>
--- a/jack-django/register.xlsx
+++ b/jack-django/register.xlsx
@@ -1,62 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\jack-django\jack-django\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DF5A8B-9C1B-4FB8-AD6C-B3D9B408D58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Test"/>
+    <sheet name="Test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Mobile no.</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Roll no.</t>
-  </si>
-  <si>
-    <t>SAHIL</t>
-  </si>
-  <si>
-    <t>9347151331</t>
-  </si>
-  <si>
-    <t>mdshaiksahil0510@gmail.com</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>CSE IOT</t>
-  </si>
-  <si>
-    <t>161023749019</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,23 +54,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -113,10 +78,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -154,71 +119,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -246,7 +211,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -269,11 +234,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -282,13 +247,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -298,7 +263,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -307,7 +272,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -316,7 +281,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -324,10 +289,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -392,65 +357,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>